<commit_message>
added loading view and rate service view. Updated old views and fixed mistakes
</commit_message>
<xml_diff>
--- a/Estilos.xlsx
+++ b/Estilos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Elemento</t>
   </si>
@@ -48,13 +48,19 @@
   </si>
   <si>
     <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>ToCheck</t>
+  </si>
+  <si>
+    <t>fae4dc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -68,6 +74,17 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,10 +107,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,9 +427,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -428,49 +496,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>